<commit_message>
Commit- 5 feb 7 PM
</commit_message>
<xml_diff>
--- a/udemy/src/main/java/com/espncricinfo/xlsx/Suite.xlsx
+++ b/udemy/src/main/java/com/espncricinfo/xlsx/Suite.xlsx
@@ -474,7 +474,7 @@
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -504,7 +504,7 @@
         <v>13</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -526,7 +526,7 @@
         <v>14</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>